<commit_message>
added hardware diagnostics and changed left and right wheel pins to make the cabling easier
</commit_message>
<xml_diff>
--- a/Go Kart Specifications V2.xlsx
+++ b/Go Kart Specifications V2.xlsx
@@ -1473,8 +1473,8 @@
   </sheetPr>
   <dimension ref="A1:S135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53:D57"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>